<commit_message>
add kafka life chat
</commit_message>
<xml_diff>
--- a/src/main/resources/invoices.xlsx
+++ b/src/main/resources/invoices.xlsx
@@ -56,10 +56,10 @@
     <t>PL73114011375851103681698194</t>
   </si>
   <si>
-    <t>https://enigeeringbucket.s3.us-east-2.amazonaws.com/invoice.JPG8401</t>
+    <t>https://enigeeringbucket.s3.us-east-2.amazonaws.com/invoice.JPG11af</t>
   </si>
   <si>
-    <t>2021-04-12</t>
+    <t>2021-04-13</t>
   </si>
   <si>
     <t>External</t>
@@ -119,7 +119,7 @@
     <col min="4" max="4" width="12.0" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.72265625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="31.90234375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="65.5625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="65.05859375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.78515625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="10.58203125" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>

<commit_message>
fix external invoices bug and assign client to project bug
</commit_message>
<xml_diff>
--- a/src/main/resources/invoices.xlsx
+++ b/src/main/resources/invoices.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Invoice number</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>External</t>
+  </si>
+  <si>
+    <t>1/03/2021asdasd</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="16.4921875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.53515625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="15.3203125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.0" customWidth="true" bestFit="true"/>
@@ -182,6 +185,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>